<commit_message>
20250929_commit this may be working code  o_0
</commit_message>
<xml_diff>
--- a/sweep_measurements.xlsx
+++ b/sweep_measurements.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Measurements" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Statistics" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,7 +18,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -25,16 +26,29 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b val="1"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="12"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFF00"/>
+        <bgColor rgb="00FFFF00"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +56,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,14 +441,1461 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:BG2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>VSG Setup Time (s)</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>VSA Setup Time (s)</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Center Frequency (GHz)</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Target Output Power (dBm)</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Servo Iterations</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Servo Settle Time (s)</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Corrected Input Power (dBm)</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Corrected Output Power (dBm)</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>VSA Output Power (dBm)</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>EVM (dB)</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>EVM Measure Time (s)</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Channel Power (dBm)</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Lower Adjacent ACLR (dB)</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Upper Adjacent ACLR (dB)</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>ACLR Measure Time (s)</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Polynomial DPD Power (dBm)</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Polynomial DPD EVM (dB)</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Polynomial DPD Measure Time (s)</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Polynomial DPD Channel Power (dBm)</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Polynomial DPD Lower Adjacent ACLR (dB)</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Polynomial DPD Upper Adjacent ACLR (dB)</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Polynomial DPD ACLR Measure Time (s)</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Polynomial DPD Total Time (s)</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>Polynomial DPD Servo Loops</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>Polynomial DPD Ext Servo Time (s)</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>Polynomial DPD K18 Servo Time (s)</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>Direct DPD Power (dBm)</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>Direct DPD EVM (dB)</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>Direct DPD Measure Time (s)</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>Direct DPD Channel Power (dBm)</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>Direct DPD Lower Adjacent ACLR (dB)</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>Direct DPD Upper Adjacent ACLR (dB)</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>Direct DPD ACLR Measure Time (s)</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>Direct DPD Total Time (s)</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>Direct DPD Servo Loops</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>Direct DPD Ext Servo Time (s)</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>Direct DPD K18 Servo Time (s)</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>GMP Power (dBm)</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>GMP EVM (dB)</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>GMP Measure Time (s)</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>GMP Channel Power (dBm)</t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>GMP Lower Adjacent ACLR (dB)</t>
+        </is>
+      </c>
+      <c r="AQ1" s="1" t="inlineStr">
+        <is>
+          <t>GMP Upper Adjacent ACLR (dB)</t>
+        </is>
+      </c>
+      <c r="AR1" s="1" t="inlineStr">
+        <is>
+          <t>GMP ACLR Measure Time (s)</t>
+        </is>
+      </c>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>GMP Total Time (s)</t>
+        </is>
+      </c>
+      <c r="AT1" s="1" t="inlineStr">
+        <is>
+          <t>GMP Servo Loops</t>
+        </is>
+      </c>
+      <c r="AU1" s="1" t="inlineStr">
+        <is>
+          <t>GMP Ext Servo Time (s)</t>
+        </is>
+      </c>
+      <c r="AV1" s="1" t="inlineStr">
+        <is>
+          <t>GMP K18 Servo Time (s)</t>
+        </is>
+      </c>
+      <c r="AW1" s="1" t="inlineStr">
+        <is>
+          <t>Total Elapsed Time (s)</t>
+        </is>
+      </c>
+      <c r="AX1" s="1" t="inlineStr">
+        <is>
+          <t>Comment</t>
+        </is>
+      </c>
+      <c r="AY1" s="1" t="inlineStr">
+        <is>
+          <t>ET Starting Delay (s)</t>
+        </is>
+      </c>
+      <c r="AZ1" s="1" t="inlineStr">
+        <is>
+          <t>ET Delay Step (s)</t>
+        </is>
+      </c>
+      <c r="BA1" s="1" t="inlineStr">
+        <is>
+          <t>ET Number of Shifts</t>
+        </is>
+      </c>
+      <c r="BB1" s="1" t="inlineStr">
+        <is>
+          <t>Baseline ET Delays (s)</t>
+        </is>
+      </c>
+      <c r="BC1" s="1" t="inlineStr">
+        <is>
+          <t>Baseline ET EVMs (dB)</t>
+        </is>
+      </c>
+      <c r="BD1" s="1" t="inlineStr">
+        <is>
+          <t>Baseline ET Total Time (s)</t>
+        </is>
+      </c>
+      <c r="BE1" s="1" t="inlineStr">
+        <is>
+          <t>Polynomial DPD ET Delays (s)</t>
+        </is>
+      </c>
+      <c r="BF1" s="1" t="inlineStr">
+        <is>
+          <t>Polynomial DPD ET EVMs (dB)</t>
+        </is>
+      </c>
+      <c r="BG1" s="1" t="inlineStr">
+        <is>
+          <t>Polynomial DPD ET Total Time (s)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="60" customHeight="1">
+      <c r="A2" t="n">
+        <v>1.206905126571655</v>
+      </c>
+      <c r="B2" t="n">
+        <v>16.60744500160217</v>
+      </c>
+      <c r="C2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D2" t="n">
+        <v>6</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1.01838755607605</v>
+      </c>
+      <c r="G2" t="n">
+        <v>-12.02701</v>
+      </c>
+      <c r="H2" t="n">
+        <v>6.428436</v>
+      </c>
+      <c r="I2" t="n">
+        <v>5.767349243</v>
+      </c>
+      <c r="J2" t="n">
+        <v>-45.99468613</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.8242642879486084</v>
+      </c>
+      <c r="L2" t="n">
+        <v>5.9101319313</v>
+      </c>
+      <c r="M2" t="n">
+        <v>-51.685072422</v>
+      </c>
+      <c r="N2" t="n">
+        <v>-52.5530304909</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0.6943986415863037</v>
+      </c>
+      <c r="P2" t="n">
+        <v>5.769393921</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>-46.00875092</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0.9887704849243164</v>
+      </c>
+      <c r="S2" t="n">
+        <v>5.91283845901</v>
+      </c>
+      <c r="T2" t="n">
+        <v>-51.5391392708</v>
+      </c>
+      <c r="U2" t="n">
+        <v>-52.5340542793</v>
+      </c>
+      <c r="V2" t="n">
+        <v>0.6866309642791748</v>
+      </c>
+      <c r="W2" t="n">
+        <v>22.39078974723816</v>
+      </c>
+      <c r="X2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>0.75724196434021</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA2" t="inlineStr"/>
+      <c r="AB2" t="inlineStr"/>
+      <c r="AC2" t="inlineStr"/>
+      <c r="AD2" t="inlineStr"/>
+      <c r="AE2" t="inlineStr"/>
+      <c r="AF2" t="inlineStr"/>
+      <c r="AG2" t="inlineStr"/>
+      <c r="AH2" t="inlineStr"/>
+      <c r="AI2" t="inlineStr"/>
+      <c r="AJ2" t="inlineStr"/>
+      <c r="AK2" t="inlineStr"/>
+      <c r="AL2" t="inlineStr"/>
+      <c r="AM2" t="inlineStr"/>
+      <c r="AN2" t="inlineStr"/>
+      <c r="AO2" t="inlineStr"/>
+      <c r="AP2" t="inlineStr"/>
+      <c r="AQ2" t="inlineStr"/>
+      <c r="AR2" t="inlineStr"/>
+      <c r="AS2" t="inlineStr"/>
+      <c r="AT2" t="inlineStr"/>
+      <c r="AU2" t="inlineStr"/>
+      <c r="AV2" t="inlineStr"/>
+      <c r="AW2" t="n">
+        <v>37.768</v>
+      </c>
+      <c r="AX2" s="2" t="inlineStr">
+        <is>
+          <t>The 5GNR waveform used in this test is a 100MHz UL 60kHz SCS 256QAM 135RB 0rbo configuration.
+This test utilizes the full 5G frame.
+The power servo is done after each DPD type to ensure accurate output power.
+The power servo uses the NRX power meter and external sensors for power servo.</t>
+        </is>
+      </c>
+      <c r="AY2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ2" t="n">
+        <v>1e-09</v>
+      </c>
+      <c r="BA2" t="n">
+        <v>14</v>
+      </c>
+      <c r="BB2" t="inlineStr">
+        <is>
+          <t>0.00e+00, 1.00e-09, 2.00e-09, 3.00e-09, 4.00e-09, 5.00e-09, 6.00e-09, 7.00e-09, 8.00e-09, 9.00e-09, 1.00e-08, 1.10e-08, 1.20e-08, 1.30e-08, 1.40e-08</t>
+        </is>
+      </c>
+      <c r="BC2" t="inlineStr">
+        <is>
+          <t>-46.00, -46.02, -46.03, -45.94, -46.00, -46.00, -45.99, -46.00, -46.00, -46.00, -45.99, -46.01, -46.00, -46.01, -46.00</t>
+        </is>
+      </c>
+      <c r="BD2" t="n">
+        <v>12.838</v>
+      </c>
+      <c r="BE2" t="inlineStr">
+        <is>
+          <t>0.00e+00, 1.00e-09, 2.00e-09, 3.00e-09, 4.00e-09, 5.00e-09, 6.00e-09, 7.00e-09, 8.00e-09, 9.00e-09, 1.00e-08, 1.10e-08, 1.20e-08, 1.30e-08, 1.40e-08</t>
+        </is>
+      </c>
+      <c r="BF2" t="inlineStr">
+        <is>
+          <t>-46.01, -46.02, -46.01, -45.99, -45.99, -45.98, -45.99, -45.99, -45.99, -45.98, -45.99, -45.99, -45.99, -45.99, -46.00</t>
+        </is>
+      </c>
+      <c r="BG2" t="n">
+        <v>12.85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B98"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Metric</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Number of Tests</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>VSG Setup Time (s) - Max</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1.206905126571655</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>VSG Setup Time (s) - Min</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1.206905126571655</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>VSG Setup Time (s) - Mean</t>
+        </is>
+      </c>
+      <c r="B5" s="4" t="n">
+        <v>1.206905126571655</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>VSA Setup Time (s) - Max</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>16.60744500160217</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>VSA Setup Time (s) - Min</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>16.60744500160217</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="inlineStr">
+        <is>
+          <t>VSA Setup Time (s) - Mean</t>
+        </is>
+      </c>
+      <c r="B8" s="4" t="n">
+        <v>16.60744500160217</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Center Frequency (GHz) - Max</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Center Frequency (GHz) - Min</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="inlineStr">
+        <is>
+          <t>Center Frequency (GHz) - Mean</t>
+        </is>
+      </c>
+      <c r="B11" s="4" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Target Output Power (dBm) - Max</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Target Output Power (dBm) - Min</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="inlineStr">
+        <is>
+          <t>Target Output Power (dBm) - Mean</t>
+        </is>
+      </c>
+      <c r="B14" s="4" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Servo Iterations - Max</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Servo Iterations - Min</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="inlineStr">
+        <is>
+          <t>Servo Iterations - Mean</t>
+        </is>
+      </c>
+      <c r="B17" s="4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Servo Settle Time (s) - Max</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>1.01838755607605</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Servo Settle Time (s) - Min</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>1.01838755607605</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="inlineStr">
+        <is>
+          <t>Servo Settle Time (s) - Mean</t>
+        </is>
+      </c>
+      <c r="B20" s="4" t="n">
+        <v>1.01838755607605</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Corrected Input Power (dBm) - Max</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>-12.02701</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Corrected Input Power (dBm) - Min</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>-12.02701</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="3" t="inlineStr">
+        <is>
+          <t>Corrected Input Power (dBm) - Mean</t>
+        </is>
+      </c>
+      <c r="B23" s="4" t="n">
+        <v>-12.02701</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Corrected Output Power (dBm) - Max</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>6.428436</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Corrected Output Power (dBm) - Min</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>6.428436</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="3" t="inlineStr">
+        <is>
+          <t>Corrected Output Power (dBm) - Mean</t>
+        </is>
+      </c>
+      <c r="B26" s="4" t="n">
+        <v>6.428436</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>VSA Output Power (dBm) - Max</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>5.767349243</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>VSA Output Power (dBm) - Min</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>5.767349243</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="3" t="inlineStr">
+        <is>
+          <t>VSA Output Power (dBm) - Mean</t>
+        </is>
+      </c>
+      <c r="B29" s="4" t="n">
+        <v>5.767349243</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>EVM (dB) - Max</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>-45.99468613</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>EVM (dB) - Min</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>-45.99468613</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="3" t="inlineStr">
+        <is>
+          <t>EVM (dB) - Mean</t>
+        </is>
+      </c>
+      <c r="B32" s="4" t="n">
+        <v>-45.99468613</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>EVM Measure Time (s) - Max</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>0.8242642879486084</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>EVM Measure Time (s) - Min</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>0.8242642879486084</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="3" t="inlineStr">
+        <is>
+          <t>EVM Measure Time (s) - Mean</t>
+        </is>
+      </c>
+      <c r="B35" s="4" t="n">
+        <v>0.8242642879486084</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Channel Power (dBm) - Max</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>5.9101319313</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Channel Power (dBm) - Min</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>5.9101319313</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="3" t="inlineStr">
+        <is>
+          <t>Channel Power (dBm) - Mean</t>
+        </is>
+      </c>
+      <c r="B38" s="4" t="n">
+        <v>5.9101319313</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Lower Adjacent ACLR (dB) - Max</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>-51.685072422</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Lower Adjacent ACLR (dB) - Min</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>-51.685072422</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="3" t="inlineStr">
+        <is>
+          <t>Lower Adjacent ACLR (dB) - Mean</t>
+        </is>
+      </c>
+      <c r="B41" s="4" t="n">
+        <v>-51.685072422</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Upper Adjacent ACLR (dB) - Max</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>-52.5530304909</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Upper Adjacent ACLR (dB) - Min</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>-52.5530304909</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="3" t="inlineStr">
+        <is>
+          <t>Upper Adjacent ACLR (dB) - Mean</t>
+        </is>
+      </c>
+      <c r="B44" s="4" t="n">
+        <v>-52.5530304909</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>ACLR Measure Time (s) - Max</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>0.6943986415863037</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>ACLR Measure Time (s) - Min</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>0.6943986415863037</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="3" t="inlineStr">
+        <is>
+          <t>ACLR Measure Time (s) - Mean</t>
+        </is>
+      </c>
+      <c r="B47" s="4" t="n">
+        <v>0.6943986415863037</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Polynomial DPD Power (dBm) - Max</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>5.769393921</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Polynomial DPD Power (dBm) - Min</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>5.769393921</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="3" t="inlineStr">
+        <is>
+          <t>Polynomial DPD Power (dBm) - Mean</t>
+        </is>
+      </c>
+      <c r="B50" s="4" t="n">
+        <v>5.769393921</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Polynomial DPD EVM (dB) - Max</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>-46.00875092</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Polynomial DPD EVM (dB) - Min</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>-46.00875092</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="3" t="inlineStr">
+        <is>
+          <t>Polynomial DPD EVM (dB) - Mean</t>
+        </is>
+      </c>
+      <c r="B53" s="4" t="n">
+        <v>-46.00875092</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Polynomial DPD Measure Time (s) - Max</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>0.9887704849243164</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Polynomial DPD Measure Time (s) - Min</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>0.9887704849243164</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="3" t="inlineStr">
+        <is>
+          <t>Polynomial DPD Measure Time (s) - Mean</t>
+        </is>
+      </c>
+      <c r="B56" s="4" t="n">
+        <v>0.9887704849243164</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Polynomial DPD Channel Power (dBm) - Max</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>5.91283845901</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Polynomial DPD Channel Power (dBm) - Min</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>5.91283845901</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="3" t="inlineStr">
+        <is>
+          <t>Polynomial DPD Channel Power (dBm) - Mean</t>
+        </is>
+      </c>
+      <c r="B59" s="4" t="n">
+        <v>5.91283845901</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Polynomial DPD Lower Adjacent ACLR (dB) - Max</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>-51.5391392708</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Polynomial DPD Lower Adjacent ACLR (dB) - Min</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>-51.5391392708</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="3" t="inlineStr">
+        <is>
+          <t>Polynomial DPD Lower Adjacent ACLR (dB) - Mean</t>
+        </is>
+      </c>
+      <c r="B62" s="4" t="n">
+        <v>-51.5391392708</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Polynomial DPD Upper Adjacent ACLR (dB) - Max</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>-52.5340542793</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Polynomial DPD Upper Adjacent ACLR (dB) - Min</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>-52.5340542793</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="3" t="inlineStr">
+        <is>
+          <t>Polynomial DPD Upper Adjacent ACLR (dB) - Mean</t>
+        </is>
+      </c>
+      <c r="B65" s="4" t="n">
+        <v>-52.5340542793</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Polynomial DPD ACLR Measure Time (s) - Max</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>0.6866309642791748</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Polynomial DPD ACLR Measure Time (s) - Min</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>0.6866309642791748</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="3" t="inlineStr">
+        <is>
+          <t>Polynomial DPD ACLR Measure Time (s) - Mean</t>
+        </is>
+      </c>
+      <c r="B68" s="4" t="n">
+        <v>0.6866309642791748</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Polynomial DPD Total Time (s) - Max</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>22.39078974723816</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Polynomial DPD Total Time (s) - Min</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>22.39078974723816</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="3" t="inlineStr">
+        <is>
+          <t>Polynomial DPD Total Time (s) - Mean</t>
+        </is>
+      </c>
+      <c r="B71" s="4" t="n">
+        <v>22.39078974723816</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Polynomial DPD Servo Loops - Max</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Polynomial DPD Servo Loops - Min</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="3" t="inlineStr">
+        <is>
+          <t>Polynomial DPD Servo Loops - Mean</t>
+        </is>
+      </c>
+      <c r="B74" s="4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Polynomial DPD Ext Servo Time (s) - Max</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>0.75724196434021</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Polynomial DPD Ext Servo Time (s) - Min</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>0.75724196434021</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="3" t="inlineStr">
+        <is>
+          <t>Polynomial DPD Ext Servo Time (s) - Mean</t>
+        </is>
+      </c>
+      <c r="B77" s="4" t="n">
+        <v>0.75724196434021</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Polynomial DPD K18 Servo Time (s) - Max</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Polynomial DPD K18 Servo Time (s) - Min</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="3" t="inlineStr">
+        <is>
+          <t>Polynomial DPD K18 Servo Time (s) - Mean</t>
+        </is>
+      </c>
+      <c r="B80" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Total Elapsed Time (s) - Max</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>37.768</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Total Elapsed Time (s) - Min</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>37.768</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="3" t="inlineStr">
+        <is>
+          <t>Total Elapsed Time (s) - Mean</t>
+        </is>
+      </c>
+      <c r="B83" s="4" t="n">
+        <v>37.768</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>ET Starting Delay (s) - Max</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>ET Starting Delay (s) - Min</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="3" t="inlineStr">
+        <is>
+          <t>ET Starting Delay (s) - Mean</t>
+        </is>
+      </c>
+      <c r="B86" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>ET Delay Step (s) - Max</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>1e-09</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>ET Delay Step (s) - Min</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
+        <v>1e-09</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="3" t="inlineStr">
+        <is>
+          <t>ET Delay Step (s) - Mean</t>
+        </is>
+      </c>
+      <c r="B89" s="4" t="n">
+        <v>1e-09</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>ET Number of Shifts - Max</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>ET Number of Shifts - Min</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="3" t="inlineStr">
+        <is>
+          <t>ET Number of Shifts - Mean</t>
+        </is>
+      </c>
+      <c r="B92" s="4" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>Baseline ET Total Time (s) - Max</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>12.838</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>Baseline ET Total Time (s) - Min</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>12.838</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="3" t="inlineStr">
+        <is>
+          <t>Baseline ET Total Time (s) - Mean</t>
+        </is>
+      </c>
+      <c r="B95" s="4" t="n">
+        <v>12.838</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>Polynomial DPD ET Total Time (s) - Max</t>
+        </is>
+      </c>
+      <c r="B96" t="n">
+        <v>12.85</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>Polynomial DPD ET Total Time (s) - Min</t>
+        </is>
+      </c>
+      <c r="B97" t="n">
+        <v>12.85</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="3" t="inlineStr">
+        <is>
+          <t>Polynomial DPD ET Total Time (s) - Mean</t>
+        </is>
+      </c>
+      <c r="B98" s="4" t="n">
+        <v>12.85</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
20250929_commit this is working code 1612
</commit_message>
<xml_diff>
--- a/sweep_measurements.xlsx
+++ b/sweep_measurements.xlsx
@@ -748,10 +748,10 @@
     </row>
     <row r="2" ht="60" customHeight="1">
       <c r="A2" t="n">
-        <v>1.206905126571655</v>
+        <v>1.230139493942261</v>
       </c>
       <c r="B2" t="n">
-        <v>16.60744500160217</v>
+        <v>16.80768704414368</v>
       </c>
       <c r="C2" t="n">
         <v>2</v>
@@ -763,64 +763,64 @@
         <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>1.01838755607605</v>
+        <v>0.6845536231994629</v>
       </c>
       <c r="G2" t="n">
-        <v>-12.02701</v>
+        <v>-12.03915</v>
       </c>
       <c r="H2" t="n">
-        <v>6.428436</v>
+        <v>6.392822</v>
       </c>
       <c r="I2" t="n">
-        <v>5.767349243</v>
+        <v>6.047246933</v>
       </c>
       <c r="J2" t="n">
-        <v>-45.99468613</v>
+        <v>-45.75321198</v>
       </c>
       <c r="K2" t="n">
-        <v>0.8242642879486084</v>
+        <v>0.838693380355835</v>
       </c>
       <c r="L2" t="n">
-        <v>5.9101319313</v>
+        <v>6.15513134003</v>
       </c>
       <c r="M2" t="n">
-        <v>-51.685072422</v>
+        <v>-51.4895620346</v>
       </c>
       <c r="N2" t="n">
-        <v>-52.5530304909</v>
+        <v>-52.3492879868</v>
       </c>
       <c r="O2" t="n">
-        <v>0.6943986415863037</v>
+        <v>0.6965670585632324</v>
       </c>
       <c r="P2" t="n">
-        <v>5.769393921</v>
+        <v>6.083156586</v>
       </c>
       <c r="Q2" t="n">
-        <v>-46.00875092</v>
+        <v>-51.17642212</v>
       </c>
       <c r="R2" t="n">
-        <v>0.9887704849243164</v>
+        <v>0.9600005149841309</v>
       </c>
       <c r="S2" t="n">
-        <v>5.91283845901</v>
+        <v>6.19470405579</v>
       </c>
       <c r="T2" t="n">
-        <v>-51.5391392708</v>
+        <v>-52.3015956879</v>
       </c>
       <c r="U2" t="n">
-        <v>-52.5340542793</v>
+        <v>-53.7921848297</v>
       </c>
       <c r="V2" t="n">
-        <v>0.6866309642791748</v>
+        <v>0.6848137378692627</v>
       </c>
       <c r="W2" t="n">
-        <v>22.39078974723816</v>
+        <v>6.300565719604492</v>
       </c>
       <c r="X2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.75724196434021</v>
+        <v>1.128886699676514</v>
       </c>
       <c r="Z2" t="n">
         <v>0</v>
@@ -848,7 +848,7 @@
       <c r="AU2" t="inlineStr"/>
       <c r="AV2" t="inlineStr"/>
       <c r="AW2" t="n">
-        <v>37.768</v>
+        <v>9.385</v>
       </c>
       <c r="AX2" s="2" t="inlineStr">
         <is>
@@ -874,11 +874,11 @@
       </c>
       <c r="BC2" t="inlineStr">
         <is>
-          <t>-46.00, -46.02, -46.03, -45.94, -46.00, -46.00, -45.99, -46.00, -46.00, -46.00, -45.99, -46.01, -46.00, -46.01, -46.00</t>
+          <t>-45.75, -45.75, -45.75, -45.75, -45.75, -45.75, -45.75, -45.75, -45.75, -45.75, -45.75, -45.75, -45.75, -45.75, -45.75</t>
         </is>
       </c>
       <c r="BD2" t="n">
-        <v>12.838</v>
+        <v>0.862</v>
       </c>
       <c r="BE2" t="inlineStr">
         <is>
@@ -887,11 +887,11 @@
       </c>
       <c r="BF2" t="inlineStr">
         <is>
-          <t>-46.01, -46.02, -46.01, -45.99, -45.99, -45.98, -45.99, -45.99, -45.99, -45.98, -45.99, -45.99, -45.99, -45.99, -46.00</t>
+          <t>-51.18, -51.18, -51.18, -51.18, -51.18, -51.18, -51.18, -51.18, -51.18, -51.18, -51.18, -51.18, -51.18, -51.18, -51.18</t>
         </is>
       </c>
       <c r="BG2" t="n">
-        <v>12.85</v>
+        <v>0.862</v>
       </c>
     </row>
   </sheetData>
@@ -942,7 +942,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1.206905126571655</v>
+        <v>1.230139493942261</v>
       </c>
     </row>
     <row r="4">
@@ -952,7 +952,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1.206905126571655</v>
+        <v>1.230139493942261</v>
       </c>
     </row>
     <row r="5">
@@ -962,7 +962,7 @@
         </is>
       </c>
       <c r="B5" s="4" t="n">
-        <v>1.206905126571655</v>
+        <v>1.230139493942261</v>
       </c>
     </row>
     <row r="6">
@@ -972,7 +972,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>16.60744500160217</v>
+        <v>16.80768704414368</v>
       </c>
     </row>
     <row r="7">
@@ -982,7 +982,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>16.60744500160217</v>
+        <v>16.80768704414368</v>
       </c>
     </row>
     <row r="8">
@@ -992,7 +992,7 @@
         </is>
       </c>
       <c r="B8" s="4" t="n">
-        <v>16.60744500160217</v>
+        <v>16.80768704414368</v>
       </c>
     </row>
     <row r="9">
@@ -1092,7 +1092,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1.01838755607605</v>
+        <v>0.6845536231994629</v>
       </c>
     </row>
     <row r="19">
@@ -1102,7 +1102,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>1.01838755607605</v>
+        <v>0.6845536231994629</v>
       </c>
     </row>
     <row r="20">
@@ -1112,7 +1112,7 @@
         </is>
       </c>
       <c r="B20" s="4" t="n">
-        <v>1.01838755607605</v>
+        <v>0.6845536231994629</v>
       </c>
     </row>
     <row r="21">
@@ -1122,7 +1122,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-12.02701</v>
+        <v>-12.03915</v>
       </c>
     </row>
     <row r="22">
@@ -1132,7 +1132,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-12.02701</v>
+        <v>-12.03915</v>
       </c>
     </row>
     <row r="23">
@@ -1142,7 +1142,7 @@
         </is>
       </c>
       <c r="B23" s="4" t="n">
-        <v>-12.02701</v>
+        <v>-12.03915</v>
       </c>
     </row>
     <row r="24">
@@ -1152,7 +1152,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>6.428436</v>
+        <v>6.392822</v>
       </c>
     </row>
     <row r="25">
@@ -1162,7 +1162,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>6.428436</v>
+        <v>6.392822</v>
       </c>
     </row>
     <row r="26">
@@ -1172,7 +1172,7 @@
         </is>
       </c>
       <c r="B26" s="4" t="n">
-        <v>6.428436</v>
+        <v>6.392822</v>
       </c>
     </row>
     <row r="27">
@@ -1182,7 +1182,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>5.767349243</v>
+        <v>6.047246933</v>
       </c>
     </row>
     <row r="28">
@@ -1192,7 +1192,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>5.767349243</v>
+        <v>6.047246933</v>
       </c>
     </row>
     <row r="29">
@@ -1202,7 +1202,7 @@
         </is>
       </c>
       <c r="B29" s="4" t="n">
-        <v>5.767349243</v>
+        <v>6.047246933</v>
       </c>
     </row>
     <row r="30">
@@ -1212,7 +1212,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>-45.99468613</v>
+        <v>-45.75321198</v>
       </c>
     </row>
     <row r="31">
@@ -1222,7 +1222,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>-45.99468613</v>
+        <v>-45.75321198</v>
       </c>
     </row>
     <row r="32">
@@ -1232,7 +1232,7 @@
         </is>
       </c>
       <c r="B32" s="4" t="n">
-        <v>-45.99468613</v>
+        <v>-45.75321198</v>
       </c>
     </row>
     <row r="33">
@@ -1242,7 +1242,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.8242642879486084</v>
+        <v>0.838693380355835</v>
       </c>
     </row>
     <row r="34">
@@ -1252,7 +1252,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.8242642879486084</v>
+        <v>0.838693380355835</v>
       </c>
     </row>
     <row r="35">
@@ -1262,7 +1262,7 @@
         </is>
       </c>
       <c r="B35" s="4" t="n">
-        <v>0.8242642879486084</v>
+        <v>0.838693380355835</v>
       </c>
     </row>
     <row r="36">
@@ -1272,7 +1272,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>5.9101319313</v>
+        <v>6.15513134003</v>
       </c>
     </row>
     <row r="37">
@@ -1282,7 +1282,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>5.9101319313</v>
+        <v>6.15513134003</v>
       </c>
     </row>
     <row r="38">
@@ -1292,7 +1292,7 @@
         </is>
       </c>
       <c r="B38" s="4" t="n">
-        <v>5.9101319313</v>
+        <v>6.15513134003</v>
       </c>
     </row>
     <row r="39">
@@ -1302,7 +1302,7 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>-51.685072422</v>
+        <v>-51.4895620346</v>
       </c>
     </row>
     <row r="40">
@@ -1312,7 +1312,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>-51.685072422</v>
+        <v>-51.4895620346</v>
       </c>
     </row>
     <row r="41">
@@ -1322,7 +1322,7 @@
         </is>
       </c>
       <c r="B41" s="4" t="n">
-        <v>-51.685072422</v>
+        <v>-51.4895620346</v>
       </c>
     </row>
     <row r="42">
@@ -1332,7 +1332,7 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>-52.5530304909</v>
+        <v>-52.3492879868</v>
       </c>
     </row>
     <row r="43">
@@ -1342,7 +1342,7 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>-52.5530304909</v>
+        <v>-52.3492879868</v>
       </c>
     </row>
     <row r="44">
@@ -1352,7 +1352,7 @@
         </is>
       </c>
       <c r="B44" s="4" t="n">
-        <v>-52.5530304909</v>
+        <v>-52.3492879868</v>
       </c>
     </row>
     <row r="45">
@@ -1362,7 +1362,7 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>0.6943986415863037</v>
+        <v>0.6965670585632324</v>
       </c>
     </row>
     <row r="46">
@@ -1372,7 +1372,7 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>0.6943986415863037</v>
+        <v>0.6965670585632324</v>
       </c>
     </row>
     <row r="47">
@@ -1382,7 +1382,7 @@
         </is>
       </c>
       <c r="B47" s="4" t="n">
-        <v>0.6943986415863037</v>
+        <v>0.6965670585632324</v>
       </c>
     </row>
     <row r="48">
@@ -1392,7 +1392,7 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>5.769393921</v>
+        <v>6.083156586</v>
       </c>
     </row>
     <row r="49">
@@ -1402,7 +1402,7 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>5.769393921</v>
+        <v>6.083156586</v>
       </c>
     </row>
     <row r="50">
@@ -1412,7 +1412,7 @@
         </is>
       </c>
       <c r="B50" s="4" t="n">
-        <v>5.769393921</v>
+        <v>6.083156586</v>
       </c>
     </row>
     <row r="51">
@@ -1422,7 +1422,7 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>-46.00875092</v>
+        <v>-51.17642212</v>
       </c>
     </row>
     <row r="52">
@@ -1432,7 +1432,7 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>-46.00875092</v>
+        <v>-51.17642212</v>
       </c>
     </row>
     <row r="53">
@@ -1442,7 +1442,7 @@
         </is>
       </c>
       <c r="B53" s="4" t="n">
-        <v>-46.00875092</v>
+        <v>-51.17642212</v>
       </c>
     </row>
     <row r="54">
@@ -1452,7 +1452,7 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>0.9887704849243164</v>
+        <v>0.9600005149841309</v>
       </c>
     </row>
     <row r="55">
@@ -1462,7 +1462,7 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>0.9887704849243164</v>
+        <v>0.9600005149841309</v>
       </c>
     </row>
     <row r="56">
@@ -1472,7 +1472,7 @@
         </is>
       </c>
       <c r="B56" s="4" t="n">
-        <v>0.9887704849243164</v>
+        <v>0.9600005149841309</v>
       </c>
     </row>
     <row r="57">
@@ -1482,7 +1482,7 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>5.91283845901</v>
+        <v>6.19470405579</v>
       </c>
     </row>
     <row r="58">
@@ -1492,7 +1492,7 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>5.91283845901</v>
+        <v>6.19470405579</v>
       </c>
     </row>
     <row r="59">
@@ -1502,7 +1502,7 @@
         </is>
       </c>
       <c r="B59" s="4" t="n">
-        <v>5.91283845901</v>
+        <v>6.19470405579</v>
       </c>
     </row>
     <row r="60">
@@ -1512,7 +1512,7 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>-51.5391392708</v>
+        <v>-52.3015956879</v>
       </c>
     </row>
     <row r="61">
@@ -1522,7 +1522,7 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>-51.5391392708</v>
+        <v>-52.3015956879</v>
       </c>
     </row>
     <row r="62">
@@ -1532,7 +1532,7 @@
         </is>
       </c>
       <c r="B62" s="4" t="n">
-        <v>-51.5391392708</v>
+        <v>-52.3015956879</v>
       </c>
     </row>
     <row r="63">
@@ -1542,7 +1542,7 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>-52.5340542793</v>
+        <v>-53.7921848297</v>
       </c>
     </row>
     <row r="64">
@@ -1552,7 +1552,7 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>-52.5340542793</v>
+        <v>-53.7921848297</v>
       </c>
     </row>
     <row r="65">
@@ -1562,7 +1562,7 @@
         </is>
       </c>
       <c r="B65" s="4" t="n">
-        <v>-52.5340542793</v>
+        <v>-53.7921848297</v>
       </c>
     </row>
     <row r="66">
@@ -1572,7 +1572,7 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>0.6866309642791748</v>
+        <v>0.6848137378692627</v>
       </c>
     </row>
     <row r="67">
@@ -1582,7 +1582,7 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>0.6866309642791748</v>
+        <v>0.6848137378692627</v>
       </c>
     </row>
     <row r="68">
@@ -1592,7 +1592,7 @@
         </is>
       </c>
       <c r="B68" s="4" t="n">
-        <v>0.6866309642791748</v>
+        <v>0.6848137378692627</v>
       </c>
     </row>
     <row r="69">
@@ -1602,7 +1602,7 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>22.39078974723816</v>
+        <v>6.300565719604492</v>
       </c>
     </row>
     <row r="70">
@@ -1612,7 +1612,7 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>22.39078974723816</v>
+        <v>6.300565719604492</v>
       </c>
     </row>
     <row r="71">
@@ -1622,7 +1622,7 @@
         </is>
       </c>
       <c r="B71" s="4" t="n">
-        <v>22.39078974723816</v>
+        <v>6.300565719604492</v>
       </c>
     </row>
     <row r="72">
@@ -1632,7 +1632,7 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="73">
@@ -1642,7 +1642,7 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="74">
@@ -1652,7 +1652,7 @@
         </is>
       </c>
       <c r="B74" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="75">
@@ -1662,7 +1662,7 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>0.75724196434021</v>
+        <v>1.128886699676514</v>
       </c>
     </row>
     <row r="76">
@@ -1672,7 +1672,7 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>0.75724196434021</v>
+        <v>1.128886699676514</v>
       </c>
     </row>
     <row r="77">
@@ -1682,7 +1682,7 @@
         </is>
       </c>
       <c r="B77" s="4" t="n">
-        <v>0.75724196434021</v>
+        <v>1.128886699676514</v>
       </c>
     </row>
     <row r="78">
@@ -1722,7 +1722,7 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>37.768</v>
+        <v>9.385</v>
       </c>
     </row>
     <row r="82">
@@ -1732,7 +1732,7 @@
         </is>
       </c>
       <c r="B82" t="n">
-        <v>37.768</v>
+        <v>9.385</v>
       </c>
     </row>
     <row r="83">
@@ -1742,7 +1742,7 @@
         </is>
       </c>
       <c r="B83" s="4" t="n">
-        <v>37.768</v>
+        <v>9.385</v>
       </c>
     </row>
     <row r="84">
@@ -1842,7 +1842,7 @@
         </is>
       </c>
       <c r="B93" t="n">
-        <v>12.838</v>
+        <v>0.862</v>
       </c>
     </row>
     <row r="94">
@@ -1852,7 +1852,7 @@
         </is>
       </c>
       <c r="B94" t="n">
-        <v>12.838</v>
+        <v>0.862</v>
       </c>
     </row>
     <row r="95">
@@ -1862,7 +1862,7 @@
         </is>
       </c>
       <c r="B95" s="4" t="n">
-        <v>12.838</v>
+        <v>0.862</v>
       </c>
     </row>
     <row r="96">
@@ -1872,7 +1872,7 @@
         </is>
       </c>
       <c r="B96" t="n">
-        <v>12.85</v>
+        <v>0.862</v>
       </c>
     </row>
     <row r="97">
@@ -1882,7 +1882,7 @@
         </is>
       </c>
       <c r="B97" t="n">
-        <v>12.85</v>
+        <v>0.862</v>
       </c>
     </row>
     <row r="98">
@@ -1892,7 +1892,7 @@
         </is>
       </c>
       <c r="B98" s="4" t="n">
-        <v>12.85</v>
+        <v>0.862</v>
       </c>
     </row>
   </sheetData>

</xml_diff>